<commit_message>
add the original paper
</commit_message>
<xml_diff>
--- a/summary/Robot Schedule.xlsx
+++ b/summary/Robot Schedule.xlsx
@@ -23,9 +23,6 @@
     <t>HOURS</t>
   </si>
   <si>
-    <t>TOTAL</t>
-  </si>
-  <si>
     <t>Week 2</t>
   </si>
   <si>
@@ -81,6 +78,9 @@
   </si>
   <si>
     <t>Test and clean code</t>
+  </si>
+  <si>
+    <t>Totoal</t>
   </si>
 </sst>
 </file>
@@ -95,6 +95,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -154,8 +155,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -180,10 +185,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -200,38 +205,32 @@
       <c r="C1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="0" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>4</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="n">
-        <f aca="false">SUM(C2:C16)</f>
-        <v>26</v>
-      </c>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="0" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
       <c r="B4" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>1</v>
@@ -240,47 +239,47 @@
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
       <c r="B5" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>9</v>
-      </c>
       <c r="C6" s="0" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>12</v>
-      </c>
       <c r="C8" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1"/>
       <c r="B9" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>3</v>
@@ -289,7 +288,7 @@
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1"/>
       <c r="B10" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>1</v>
@@ -297,44 +296,53 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="C11" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="0" t="s">
-        <v>18</v>
-      </c>
       <c r="C12" s="0" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1"/>
       <c r="B13" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="1" t="n">
-        <v>3</v>
+      <c r="C17" s="0" t="n">
+        <f aca="false">SUM(C2:C16)</f>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>